<commit_message>
Update IATA Dynamic Region
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_IATAID02/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_IATAID02/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_IATAID02\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB680F68-0CD6-45AA-A417-88D4AC8FC38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F01842-8761-4078-B976-8C6E3694FFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23232" windowHeight="11496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>PathTabula</t>
+  </si>
+  <si>
+    <t>PathTemplateIata</t>
+  </si>
+  <si>
+    <t>Data\Template\Template_IATA.xlsx</t>
   </si>
 </sst>
 </file>
@@ -640,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -767,7 +773,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.3" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.3" customHeight="1"/>
@@ -2928,7 +2941,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update mail raw & adjustment for deployment
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_IATAID02/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_IATAID02/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_IATAID02\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F01842-8761-4078-B976-8C6E3694FFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9ED384-C98F-4A69-8FC0-92ED3B230C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -185,9 +185,6 @@
     <t>PathSAKey</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_UploadBucket</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -197,21 +194,6 @@
     <t>DialogDownloadChrome</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_PathDownloadChrome</t>
-  </si>
-  <si>
-    <t>[Dev] RPA_Moon_DialogDownloadChrome</t>
-  </si>
-  <si>
     <t>SenderName</t>
   </si>
   <si>
@@ -221,9 +203,6 @@
     <t>RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
-  </si>
-  <si>
     <t>IATACalendarURL</t>
   </si>
   <si>
@@ -248,9 +227,6 @@
     <t>https://portal.iata.org/s/</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_PathTabula</t>
-  </si>
-  <si>
     <t>PathTabula</t>
   </si>
   <si>
@@ -258,6 +234,102 @@
   </si>
   <si>
     <t>Data\Template\Template_IATA.xlsx</t>
+  </si>
+  <si>
+    <t>RPA132_IATA_ID02_MailRawTo</t>
+  </si>
+  <si>
+    <t>RPA132_IATA_ID02_MailRawCc</t>
+  </si>
+  <si>
+    <t>RPA133_IATA_MY02_MailRawTo</t>
+  </si>
+  <si>
+    <t>RPA133_IATA_MY02_MailRawCc</t>
+  </si>
+  <si>
+    <t>RPA134_IATA_SG02_MailRawTo</t>
+  </si>
+  <si>
+    <t>RPA134_IATA_SG02_MailRawCc</t>
+  </si>
+  <si>
+    <t>RPA135_IATA_MY12_MailRawTo</t>
+  </si>
+  <si>
+    <t>RPA135_IATA_MY12_MailRawCc</t>
+  </si>
+  <si>
+    <t>RPA136_IATA_TH02_MailRawTo</t>
+  </si>
+  <si>
+    <t>RPA136_IATA_TH02_MailRawCc</t>
+  </si>
+  <si>
+    <t>RPA137_IATA_VN02_MailRawTo</t>
+  </si>
+  <si>
+    <t>RPA137_IATA_VN02_MailRawCc</t>
+  </si>
+  <si>
+    <t>IATAID02_MailRawTo</t>
+  </si>
+  <si>
+    <t>IATAID02_MailRawCc</t>
+  </si>
+  <si>
+    <t>IATAMY02_MailRawTo</t>
+  </si>
+  <si>
+    <t>IATAMY02_MailRawCc</t>
+  </si>
+  <si>
+    <t>IATASG02_MailRawTo</t>
+  </si>
+  <si>
+    <t>IATASG02_MailRawCc</t>
+  </si>
+  <si>
+    <t>IATAMY12_MailRawTo</t>
+  </si>
+  <si>
+    <t>IATAMY12_MailRawCc</t>
+  </si>
+  <si>
+    <t>IATATH02_MailRawTo</t>
+  </si>
+  <si>
+    <t>IATATH02_MailRawCc</t>
+  </si>
+  <si>
+    <t>IATAVN02_MailRawTo</t>
+  </si>
+  <si>
+    <t>IATAVN02_MailRawCc</t>
+  </si>
+  <si>
+    <t>RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
+    <t>RPA_Moon_SheetIdConfig_Transport</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA_Moon_DialogDownloadChrome</t>
+  </si>
+  <si>
+    <t>RPA_Moon_PathTabula</t>
   </si>
 </sst>
 </file>
@@ -348,9 +420,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -388,7 +460,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -494,7 +566,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -636,7 +708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -646,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -694,10 +766,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.3" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -735,7 +807,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -743,42 +815,42 @@
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.3" customHeight="1">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.3" customHeight="1">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.3" customHeight="1">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.3" customHeight="1"/>
@@ -2941,8 +3013,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2994,7 +3066,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -3002,7 +3074,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -3010,7 +3082,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -3018,64 +3090,148 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
       <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="17" ht="14.3" customHeight="1"/>
-    <row r="18" ht="14.3" customHeight="1"/>
-    <row r="19" ht="14.3" customHeight="1"/>
-    <row r="20" ht="14.3" customHeight="1"/>
-    <row r="21" ht="14.3" customHeight="1"/>
-    <row r="22" ht="14.3" customHeight="1"/>
-    <row r="23" ht="14.3" customHeight="1"/>
-    <row r="24" ht="14.3" customHeight="1"/>
-    <row r="25" ht="14.3" customHeight="1"/>
-    <row r="26" ht="14.3" customHeight="1"/>
-    <row r="27" ht="14.3" customHeight="1"/>
-    <row r="28" ht="14.3" customHeight="1"/>
-    <row r="29" ht="14.3" customHeight="1"/>
-    <row r="30" ht="14.3" customHeight="1"/>
-    <row r="31" ht="14.3" customHeight="1"/>
-    <row r="32" ht="14.3" customHeight="1"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.3" customHeight="1">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.3" customHeight="1">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.3" customHeight="1">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.3" customHeight="1">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.3" customHeight="1">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.3" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.3" customHeight="1"/>
     <row r="33" ht="14.3" customHeight="1"/>
     <row r="34" ht="14.3" customHeight="1"/>
     <row r="35" ht="14.3" customHeight="1"/>

</xml_diff>